<commit_message>
modificados los estilos en el listado de alternativas y cómo se mostraba la información
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosyanez/Documents/lista-cb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8CF1C5-1C85-8148-86F9-6B1CF3843293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A24C268-F0DD-054C-A1CB-4571BAD1BE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{7C1CB140-3D0A-7D4F-AA37-4F2BBC3134C1}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$BO$1:$CC$272</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$CC$274</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3293" uniqueCount="1171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3305" uniqueCount="1172">
   <si>
     <t>cb</t>
   </si>
@@ -3553,6 +3553,9 @@
   </si>
   <si>
     <t>F-1492</t>
+  </si>
+  <si>
+    <t>HIDRORONOL-T COM X 60</t>
   </si>
 </sst>
 </file>
@@ -4016,11 +4019,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C510029-7A77-F34A-8A28-8CDA7E85138F}">
-  <dimension ref="A1:CC273"/>
+  <dimension ref="A1:CC274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF187" sqref="AF187:CB188"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BO1" sqref="BO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -60812,7 +60815,7 @@
       <c r="AD271" s="1"/>
       <c r="AE271" s="4"/>
       <c r="AF271" t="str">
-        <f t="shared" ref="AF271:AF273" si="803">+E271</f>
+        <f t="shared" ref="AF271:AF274" si="803">+E271</f>
         <v>DULOXETINA CAP 60 MG X 30</v>
       </c>
       <c r="AG271" t="str">
@@ -60844,7 +60847,7 @@
         <v>DULOXETINA CAP 60 MG X 30 SEVEN PHARMA DULOXETINA 60 MG cápsula</v>
       </c>
       <c r="BB271">
-        <f t="shared" ref="BB271:BB273" si="810">+D271</f>
+        <f t="shared" ref="BB271:BB274" si="810">+D271</f>
         <v>830565</v>
       </c>
       <c r="BC271" t="str">
@@ -60888,7 +60891,7 @@
         <v>ud.</v>
       </c>
       <c r="BO271">
-        <f t="shared" ref="BO271:BO273" si="820">+BB271</f>
+        <f t="shared" ref="BO271:BO274" si="820">+BB271</f>
         <v>830565</v>
       </c>
       <c r="BP271" t="str">
@@ -61323,8 +61326,209 @@
         <v>1</v>
       </c>
     </row>
+    <row r="274" spans="4:80" x14ac:dyDescent="0.2">
+      <c r="D274">
+        <v>831267</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F274" s="1" t="str">
+        <f t="shared" ref="F274" si="831">+MID(E274,1,FIND(Q274,E274,1)-2)</f>
+        <v>HIDRORONOL-T</v>
+      </c>
+      <c r="G274" s="1" t="str">
+        <f t="shared" ref="G274" si="832">+R274</f>
+        <v>25/50</v>
+      </c>
+      <c r="H274" s="16" t="str">
+        <f t="shared" ref="H274" si="833">+IF(LEFT(F274,4)="(CB)",PROPER(RIGHT(F274,LEN(F274)-5))&amp;" "&amp;G274,PROPER(RIGHT(F274,LEN(F274)))&amp;" "&amp;G274)</f>
+        <v>Hidroronol-T 25/50</v>
+      </c>
+      <c r="I274" s="1" t="str">
+        <f>+VLOOKUP(Q274,Hoja2!A:B,2,0)</f>
+        <v>comprimido</v>
+      </c>
+      <c r="J274" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="K274" s="1" t="str">
+        <f t="shared" ref="K274" si="834">PROPER(J274)</f>
+        <v>Itf Labomed</v>
+      </c>
+      <c r="L274" s="1" t="s">
+        <v>1164</v>
+      </c>
+      <c r="M274" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="N274" s="1" t="s">
+        <v>1165</v>
+      </c>
+      <c r="O274" s="1"/>
+      <c r="P274" s="1" t="s">
+        <v>1167</v>
+      </c>
+      <c r="Q274" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R274" s="1" t="s">
+        <v>1168</v>
+      </c>
+      <c r="S274" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T274" s="1" t="s">
+        <v>1169</v>
+      </c>
+      <c r="U274" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="V274" s="1"/>
+      <c r="W274" s="1">
+        <v>60</v>
+      </c>
+      <c r="X274" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y274" t="str">
+        <f>+IF(AND(X274="ud.",COUNTIF(Hoja2!$I$3:$I$11,Hoja1!Q274)&gt;0),Hoja1!W274&amp;" "&amp;IF(Hoja1!W274=1,VLOOKUP(Hoja1!Q274,Hoja2!$A:$D,3,0),VLOOKUP(Hoja1!Q274,Hoja2!$A:$D,4,0)),IF(AND(X274="ud.",COUNTIF(Hoja2!$I$3:$I$11,Hoja1!Q274)&lt;0),Hoja1!W274&amp;" "&amp;"unidad, "&amp;VLOOKUP(Hoja1!Q274,Hoja2!$A:$B,2,0),Hoja1!W274&amp;" "&amp;Hoja1!X274&amp;" "&amp;VLOOKUP(Hoja1!Q274,Hoja2!$A:$B,2,0)))</f>
+        <v>60 comprimidos</v>
+      </c>
+      <c r="Z274" t="str">
+        <f>+IF(X274="ud.",IF(W274&lt;&gt;1,W274&amp;" "&amp;VLOOKUP(Q274,Hoja2!A:D,4,0),Hoja1!W274&amp;" "&amp;VLOOKUP(Hoja1!Q274,Hoja2!A:D,3,0)),Hoja1!W274&amp;" "&amp;Hoja1!X274&amp;" "&amp;VLOOKUP(Hoja1!Q274,Hoja2!A:B,2,0))</f>
+        <v>60 comprimidos</v>
+      </c>
+      <c r="AA274" s="1"/>
+      <c r="AB274" s="1"/>
+      <c r="AC274" s="1"/>
+      <c r="AD274" s="1"/>
+      <c r="AE274" s="4"/>
+      <c r="AF274" t="str">
+        <f t="shared" ref="AF274" si="835">+E274</f>
+        <v>HIDRORONOL-T COM X 60</v>
+      </c>
+      <c r="AG274" t="str">
+        <f t="shared" ref="AG274" si="836">+J274</f>
+        <v>ITF LABOMED</v>
+      </c>
+      <c r="AH274" t="str">
+        <f t="shared" ref="AH274" si="837">+M274&amp;" "&amp;T274</f>
+        <v>HIDROCLOROTIAZIDA 25 MG</v>
+      </c>
+      <c r="AI274" t="str">
+        <f t="shared" ref="AI274" si="838">+IF(N274="","",N274&amp;" "&amp;U274)</f>
+        <v>TRIAMTERENO 50 MG</v>
+      </c>
+      <c r="AJ274" t="str">
+        <f t="shared" ref="AJ274" si="839">+IF(O274="","",O274&amp;" "&amp;V274)</f>
+        <v/>
+      </c>
+      <c r="AK274" t="str">
+        <f t="shared" ref="AK274" si="840">+IF(AND(AI274="",AJ274=""),AH274,IF(AND(AJ274="",AI274&lt;&gt;""),AH274&amp;" "&amp;AI274,AH274&amp;" "&amp;AI274&amp;" "&amp;AJ274))</f>
+        <v>HIDROCLOROTIAZIDA 25 MG TRIAMTERENO 50 MG</v>
+      </c>
+      <c r="AL274" t="str">
+        <f>+VLOOKUP($Q274,Hoja2!$A:$B,2,0)</f>
+        <v>comprimido</v>
+      </c>
+      <c r="AM274" t="str">
+        <f t="shared" ref="AM274" si="841">+AF274&amp;" "&amp;AG274&amp;" "&amp;AK274&amp;" "&amp;AL274</f>
+        <v>HIDRORONOL-T COM X 60 ITF LABOMED HIDROCLOROTIAZIDA 25 MG TRIAMTERENO 50 MG comprimido</v>
+      </c>
+      <c r="BB274">
+        <f t="shared" ref="BB274" si="842">+D274</f>
+        <v>831267</v>
+      </c>
+      <c r="BC274" t="str">
+        <f t="shared" ref="BC274" si="843">+H274&amp;" "&amp;IF(S274="","x ",S274&amp;" x ")&amp;Y274</f>
+        <v>Hidroronol-T 25/50 mg x 60 comprimidos</v>
+      </c>
+      <c r="BD274" s="10">
+        <f t="shared" ref="BD274" si="844">+AE274</f>
+        <v>0</v>
+      </c>
+      <c r="BE274" s="3" t="str">
+        <f t="shared" ref="BE274" si="845">+H274</f>
+        <v>Hidroronol-T 25/50</v>
+      </c>
+      <c r="BF274" t="str">
+        <f t="shared" ref="BF274" si="846">+PROPER(M274)</f>
+        <v>Hidroclorotiazida</v>
+      </c>
+      <c r="BG274" t="str">
+        <f t="shared" ref="BG274" si="847">+PROPER(N274)</f>
+        <v>Triamtereno</v>
+      </c>
+      <c r="BH274" t="str">
+        <f t="shared" ref="BH274" si="848">+PROPER(O274)</f>
+        <v/>
+      </c>
+      <c r="BI274" t="str">
+        <f>+IF(AND(X274="ud.",COUNTIF(Hoja2!$I$3:$I$11,Hoja1!Q274)&gt;0),IF(Hoja1!W274=1,VLOOKUP(Hoja1!Q274,Hoja2!$A:$D,3,0),VLOOKUP(Hoja1!Q274,Hoja2!$A:$D,4,0)),IF(AND(X274="ud.",COUNTIF(Hoja2!$I$3:$I$11,Hoja1!Q274)&lt;0),VLOOKUP(Hoja1!Q274,Hoja2!$A:$B,2,0),VLOOKUP(Hoja1!Q274,Hoja2!$A:$B,2,0)))</f>
+        <v>comprimidos</v>
+      </c>
+      <c r="BJ274" t="str">
+        <f t="shared" ref="BJ274" si="849">+G274&amp;" "&amp;S274</f>
+        <v>25/50 mg</v>
+      </c>
+      <c r="BK274">
+        <f t="shared" ref="BK274" si="850">+W274</f>
+        <v>60</v>
+      </c>
+      <c r="BL274" t="str">
+        <f t="shared" ref="BL274" si="851">+X274</f>
+        <v>ud.</v>
+      </c>
+      <c r="BO274">
+        <f t="shared" ref="BO274" si="852">+BB274</f>
+        <v>831267</v>
+      </c>
+      <c r="BP274" t="str">
+        <f t="shared" ref="BP274" si="853">+BC274</f>
+        <v>Hidroronol-T 25/50 mg x 60 comprimidos</v>
+      </c>
+      <c r="BQ274" s="10">
+        <f t="shared" ref="BQ274" si="854">+BD274</f>
+        <v>0</v>
+      </c>
+      <c r="BR274" s="3" t="str">
+        <f t="shared" ref="BR274" si="855">+BE274</f>
+        <v>Hidroronol-T 25/50</v>
+      </c>
+      <c r="BS274" t="str">
+        <f t="shared" ref="BS274" si="856">+IF(AND(BG274="",BH274=""),BF274,IF(AND(BG274&lt;&gt;"",BH274=""),BF274&amp;";"&amp;BG274,BF274&amp;";"&amp;BG274&amp;";"&amp;BH274))</f>
+        <v>Hidroclorotiazida;Triamtereno</v>
+      </c>
+      <c r="BT274" t="str">
+        <f t="shared" ref="BT274" si="857">+BI274</f>
+        <v>comprimidos</v>
+      </c>
+      <c r="BU274" t="str">
+        <f t="shared" ref="BU274" si="858">+BJ274</f>
+        <v>25/50 mg</v>
+      </c>
+      <c r="BV274">
+        <f t="shared" ref="BV274" si="859">+BK274</f>
+        <v>60</v>
+      </c>
+      <c r="BW274" t="str">
+        <f t="shared" ref="BW274" si="860">+BL274</f>
+        <v>ud.</v>
+      </c>
+      <c r="BZ274" t="str">
+        <f t="shared" ref="BZ274" si="861">+K274</f>
+        <v>Itf Labomed</v>
+      </c>
+      <c r="CB274">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="BO1:CC272" xr:uid="{6C510029-7A77-F34A-8A28-8CDA7E85138F}"/>
+  <autoFilter ref="A1:CC274" xr:uid="{6C510029-7A77-F34A-8A28-8CDA7E85138F}">
+    <filterColumn colId="57" showButton="0"/>
+    <filterColumn colId="58" showButton="0"/>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="BF1:BH1"/>
   </mergeCells>

</xml_diff>

<commit_message>
actualiza base y elimina precio de alternativas
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosyanez/Documents/lista-cb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64C56D7-FF2F-8147-A151-CEC30628A359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AA47E1-401C-2147-880B-D042D8DF9A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17620" xr2:uid="{7C1CB140-3D0A-7D4F-AA37-4F2BBC3134C1}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$CC$276</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$CC$280</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3371" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3381" uniqueCount="1193">
   <si>
     <t>cb</t>
   </si>
@@ -3610,6 +3610,15 @@
   </si>
   <si>
     <t>VANNAIR SUS INH ORA 160/4,5 MG X 120 DSS</t>
+  </si>
+  <si>
+    <t>ADAPAC GEL TOP 0,1% X 30 GR</t>
+  </si>
+  <si>
+    <t>832188;833801</t>
+  </si>
+  <si>
+    <t>830932;1709585</t>
   </si>
 </sst>
 </file>
@@ -4073,11 +4082,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C510029-7A77-F34A-8A28-8CDA7E85138F}">
-  <dimension ref="A1:CC279"/>
+  <dimension ref="A1:CC280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BJ1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BX278" sqref="BX278"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="CB280" sqref="CB280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12052,6 +12061,9 @@
         <f t="shared" si="32"/>
         <v>Novartis</v>
       </c>
+      <c r="CA37">
+        <v>1713821</v>
+      </c>
       <c r="CB37">
         <v>0</v>
       </c>
@@ -17457,8 +17469,8 @@
         <f t="shared" si="32"/>
         <v>Global Pharma</v>
       </c>
-      <c r="CA62">
-        <v>830932</v>
+      <c r="CA62" t="s">
+        <v>1192</v>
       </c>
       <c r="CB62">
         <v>0</v>
@@ -19199,8 +19211,8 @@
         <f t="shared" si="85"/>
         <v>Astrazeneca</v>
       </c>
-      <c r="CA70">
-        <v>832188</v>
+      <c r="CA70" t="s">
+        <v>1191</v>
       </c>
       <c r="CB70">
         <v>0</v>
@@ -41322,6 +41334,9 @@
         <f t="shared" si="139"/>
         <v>Galenicum</v>
       </c>
+      <c r="CA172">
+        <v>1713821</v>
+      </c>
       <c r="CB172">
         <v>0</v>
       </c>
@@ -44693,19 +44708,19 @@
         <v>3990</v>
       </c>
       <c r="AF188" t="str">
-        <f t="shared" ref="AF188:AF190" si="239">+E188</f>
+        <f t="shared" ref="AF188" si="239">+E188</f>
         <v>(CB) HIDRORONOL-T COM X 60</v>
       </c>
       <c r="AG188" t="str">
-        <f t="shared" ref="AG188:AG190" si="240">+J188</f>
+        <f t="shared" ref="AG188" si="240">+J188</f>
         <v>ITF LABOMED</v>
       </c>
       <c r="AH188" t="str">
-        <f t="shared" ref="AH188:AH189" si="241">+M188&amp;" "&amp;T188</f>
+        <f t="shared" ref="AH188" si="241">+M188&amp;" "&amp;T188</f>
         <v>HIDROCLOROTIAZIDA 25 MG</v>
       </c>
       <c r="AI188" t="str">
-        <f t="shared" ref="AI188:AI189" si="242">+IF(N188="","",N188&amp;" "&amp;U188)</f>
+        <f t="shared" ref="AI188" si="242">+IF(N188="","",N188&amp;" "&amp;U188)</f>
         <v>TRIAMTERENO 50 MG</v>
       </c>
       <c r="AJ188" t="str">
@@ -44741,11 +44756,11 @@
         <v>Hidroronol-T 25/50</v>
       </c>
       <c r="BF188" t="str">
-        <f t="shared" ref="BF188:BF189" si="250">+PROPER(M188)</f>
+        <f t="shared" ref="BF188" si="250">+PROPER(M188)</f>
         <v>Hidroclorotiazida</v>
       </c>
       <c r="BG188" t="str">
-        <f t="shared" ref="BG188:BG189" si="251">+PROPER(N188)</f>
+        <f t="shared" ref="BG188" si="251">+PROPER(N188)</f>
         <v>Triamtereno</v>
       </c>
       <c r="BH188" t="str">
@@ -44761,11 +44776,11 @@
         <v>25/50 mg</v>
       </c>
       <c r="BK188">
-        <f t="shared" ref="BK188:BK190" si="254">+W188</f>
+        <f t="shared" ref="BK188" si="254">+W188</f>
         <v>60</v>
       </c>
       <c r="BL188" t="str">
-        <f t="shared" ref="BL188:BL190" si="255">+X188</f>
+        <f t="shared" ref="BL188" si="255">+X188</f>
         <v>ud.</v>
       </c>
       <c r="BO188">
@@ -44797,19 +44812,19 @@
         <v>25/50 mg</v>
       </c>
       <c r="BV188">
-        <f t="shared" ref="BV188:BV190" si="263">+BK188</f>
+        <f t="shared" ref="BV188" si="263">+BK188</f>
         <v>60</v>
       </c>
       <c r="BW188" t="str">
-        <f t="shared" ref="BW188:BW190" si="264">+BL188</f>
+        <f t="shared" ref="BW188" si="264">+BL188</f>
         <v>ud.</v>
       </c>
       <c r="BZ188" t="str">
-        <f t="shared" ref="BZ188:BZ190" si="265">+K188</f>
+        <f t="shared" ref="BZ188" si="265">+K188</f>
         <v>Itf Labomed</v>
       </c>
       <c r="CA188">
-        <v>832049</v>
+        <v>831267</v>
       </c>
       <c r="CB188">
         <v>0</v>
@@ -45157,7 +45172,7 @@
         <v>Meprokem 50 mg x 30 comprimidos de liberación prolongada</v>
       </c>
       <c r="BD190" s="10">
-        <f t="shared" ref="BD189:BD190" si="291">+AE190</f>
+        <f t="shared" ref="BD190" si="291">+AE190</f>
         <v>14380</v>
       </c>
       <c r="BE190" s="3" t="str">
@@ -45201,7 +45216,7 @@
         <v>Meprokem 50 mg x 30 comprimidos de liberación prolongada</v>
       </c>
       <c r="BQ190" s="10">
-        <f t="shared" ref="BQ189:BQ190" si="292">+BD190</f>
+        <f t="shared" ref="BQ190" si="292">+BD190</f>
         <v>14380</v>
       </c>
       <c r="BR190" s="3" t="str">
@@ -45231,9 +45246,6 @@
       <c r="BZ190" t="str">
         <f t="shared" si="290"/>
         <v>Ascend</v>
-      </c>
-      <c r="CA190">
-        <v>832049</v>
       </c>
       <c r="CB190">
         <v>0</v>
@@ -61812,7 +61824,7 @@
         <v>1171</v>
       </c>
       <c r="F276" s="1" t="str">
-        <f t="shared" ref="F276:F279" si="858">+MID(E276,1,FIND(Q276,E276,1)-2)</f>
+        <f t="shared" ref="F276:F280" si="858">+MID(E276,1,FIND(Q276,E276,1)-2)</f>
         <v>HIDRORONOL-T</v>
       </c>
       <c r="G276" s="1" t="str">
@@ -61831,7 +61843,7 @@
         <v>290</v>
       </c>
       <c r="K276" s="1" t="str">
-        <f t="shared" ref="K276:K279" si="861">PROPER(J276)</f>
+        <f t="shared" ref="K276:K280" si="861">PROPER(J276)</f>
         <v>Itf Labomed</v>
       </c>
       <c r="L276" s="1" t="s">
@@ -62085,7 +62097,7 @@
         <v>NOVAFEM JER X 1</v>
       </c>
       <c r="AG277" t="str">
-        <f t="shared" ref="AG277:AG278" si="890">+J277</f>
+        <f t="shared" ref="AG277" si="890">+J277</f>
         <v>SILESIA</v>
       </c>
       <c r="AH277" t="str">
@@ -62145,15 +62157,15 @@
         <v>jeringa</v>
       </c>
       <c r="BJ277" t="str">
-        <f t="shared" ref="BJ277:BJ278" si="903">+G277&amp;" "&amp;S277</f>
+        <f t="shared" ref="BJ277" si="903">+G277&amp;" "&amp;S277</f>
         <v>25/0,5 mg/0,5ml</v>
       </c>
       <c r="BK277">
-        <f t="shared" ref="BK277:BK278" si="904">+W277</f>
+        <f t="shared" ref="BK277" si="904">+W277</f>
         <v>1</v>
       </c>
       <c r="BL277" t="str">
-        <f t="shared" ref="BL277:BL278" si="905">+X277</f>
+        <f t="shared" ref="BL277" si="905">+X277</f>
         <v>ud.</v>
       </c>
       <c r="BO277">
@@ -62181,15 +62193,15 @@
         <v>jeringa</v>
       </c>
       <c r="BU277" t="str">
-        <f t="shared" ref="BU277:BU278" si="912">+BJ277</f>
+        <f t="shared" ref="BU277" si="912">+BJ277</f>
         <v>25/0,5 mg/0,5ml</v>
       </c>
       <c r="BV277">
-        <f t="shared" ref="BV277:BV278" si="913">+BK277</f>
+        <f t="shared" ref="BV277" si="913">+BK277</f>
         <v>1</v>
       </c>
       <c r="BW277" t="str">
-        <f t="shared" ref="BW277:BW278" si="914">+BL277</f>
+        <f t="shared" ref="BW277" si="914">+BL277</f>
         <v>ud.</v>
       </c>
       <c r="BZ277" t="str">
@@ -62417,7 +62429,7 @@
         <v>160/4,5</v>
       </c>
       <c r="H279" s="16" t="str">
-        <f t="shared" ref="H279" si="942">+IF(LEFT(F279,4)="(CB)",PROPER(RIGHT(F279,LEN(F279)-5))&amp;" "&amp;G279,PROPER(RIGHT(F279,LEN(F279)))&amp;" "&amp;G279)</f>
+        <f t="shared" ref="H279:H280" si="942">+IF(LEFT(F279,4)="(CB)",PROPER(RIGHT(F279,LEN(F279)-5))&amp;" "&amp;G279,PROPER(RIGHT(F279,LEN(F279)))&amp;" "&amp;G279)</f>
         <v>Vannair 160/4,5</v>
       </c>
       <c r="I279" s="1" t="str">
@@ -62478,9 +62490,7 @@
       <c r="AB279" s="1"/>
       <c r="AC279" s="1"/>
       <c r="AD279" s="1"/>
-      <c r="AE279" s="4">
-        <v>59990</v>
-      </c>
+      <c r="AE279" s="4"/>
       <c r="AF279" t="str">
         <f t="shared" si="916"/>
         <v>VANNAIR SUS INH ORA 160/4,5 MG X 120 DSS</v>
@@ -62523,7 +62533,7 @@
       </c>
       <c r="BD279" s="10">
         <f t="shared" si="924"/>
-        <v>59990</v>
+        <v>0</v>
       </c>
       <c r="BE279" s="3" t="str">
         <f t="shared" si="925"/>
@@ -62567,7 +62577,7 @@
       </c>
       <c r="BQ279" s="10">
         <f t="shared" si="934"/>
-        <v>59990</v>
+        <v>0</v>
       </c>
       <c r="BR279" s="3" t="str">
         <f t="shared" si="935"/>
@@ -62597,15 +62607,199 @@
         <f t="shared" si="941"/>
         <v>Astrazeneca</v>
       </c>
-      <c r="CA279">
-        <v>832188</v>
-      </c>
       <c r="CB279">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="4:80" x14ac:dyDescent="0.2">
+      <c r="D280">
+        <v>1709585</v>
+      </c>
+      <c r="E280" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F280" s="1" t="str">
+        <f t="shared" si="858"/>
+        <v>ADAPAC</v>
+      </c>
+      <c r="G280" s="18" t="str">
+        <f>+T280</f>
+        <v>0,1%</v>
+      </c>
+      <c r="H280" s="16" t="str">
+        <f t="shared" si="942"/>
+        <v>Adapac 0,1%</v>
+      </c>
+      <c r="I280" s="1" t="str">
+        <f>+VLOOKUP(Q280,Hoja2!A:B,2,0)</f>
+        <v>gel tópico</v>
+      </c>
+      <c r="J280" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="K280" s="1" t="str">
+        <f t="shared" si="861"/>
+        <v>D&amp;M Pharma</v>
+      </c>
+      <c r="L280" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="M280" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P280" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="Q280" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="R280" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="T280" s="5" t="s">
+        <v>987</v>
+      </c>
+      <c r="W280" s="1">
+        <v>30</v>
+      </c>
+      <c r="X280" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="Y280" t="str">
+        <f>+IF(AND(X280="ud.",COUNTIF(Hoja2!$I$3:$I$11,Hoja1!Q280)&gt;0),Hoja1!W280&amp;" "&amp;IF(Hoja1!W280=1,VLOOKUP(Hoja1!Q280,Hoja2!$A:$D,3,0),VLOOKUP(Hoja1!Q280,Hoja2!$A:$D,4,0)),IF(AND(X280="ud.",COUNTIF(Hoja2!$I$3:$I$11,Hoja1!Q280)&lt;0),Hoja1!W280&amp;" "&amp;"unidad, "&amp;VLOOKUP(Hoja1!Q280,Hoja2!$A:$B,2,0),Hoja1!W280&amp;" "&amp;Hoja1!X280&amp;" "&amp;VLOOKUP(Hoja1!Q280,Hoja2!$A:$B,2,0)))</f>
+        <v>30 g. gel tópico</v>
+      </c>
+      <c r="Z280" t="str">
+        <f>+IF(X280="ud.",IF(W280&lt;&gt;1,W280&amp;" "&amp;VLOOKUP(Q280,Hoja2!A:D,4,0),Hoja1!W280&amp;" "&amp;VLOOKUP(Hoja1!Q280,Hoja2!A:D,3,0)),Hoja1!W280&amp;" "&amp;Hoja1!X280&amp;" "&amp;VLOOKUP(Hoja1!Q280,Hoja2!A:B,2,0))</f>
+        <v>30 g. gel tópico</v>
+      </c>
+      <c r="AA280" s="1"/>
+      <c r="AB280" s="1"/>
+      <c r="AC280" s="1"/>
+      <c r="AD280" s="1"/>
+      <c r="AE280" s="4"/>
+      <c r="AF280" t="str">
+        <f t="shared" ref="AF280" si="944">+E280</f>
+        <v>ADAPAC GEL TOP 0,1% X 30 GR</v>
+      </c>
+      <c r="AG280" t="str">
+        <f t="shared" ref="AG280" si="945">+J280</f>
+        <v>D&amp;M PHARMA</v>
+      </c>
+      <c r="AH280" t="str">
+        <f t="shared" ref="AH280" si="946">+M280&amp;" "&amp;T280</f>
+        <v>ADAPALENO 0,1%</v>
+      </c>
+      <c r="AI280" t="str">
+        <f t="shared" ref="AI280" si="947">+IF(N280="","",N280&amp;" "&amp;U280)</f>
+        <v/>
+      </c>
+      <c r="AJ280" t="str">
+        <f t="shared" ref="AJ280" si="948">+IF(O280="","",O280&amp;" "&amp;V280)</f>
+        <v/>
+      </c>
+      <c r="AK280" t="str">
+        <f t="shared" ref="AK280" si="949">+IF(AND(AI280="",AJ280=""),AH280,IF(AND(AJ280="",AI280&lt;&gt;""),AH280&amp;" "&amp;AI280,AH280&amp;" "&amp;AI280&amp;" "&amp;AJ280))</f>
+        <v>ADAPALENO 0,1%</v>
+      </c>
+      <c r="AL280" t="str">
+        <f>+VLOOKUP($Q280,Hoja2!$A:$B,2,0)</f>
+        <v>gel tópico</v>
+      </c>
+      <c r="AM280" t="str">
+        <f t="shared" ref="AM280" si="950">+AF280&amp;" "&amp;AG280&amp;" "&amp;AK280&amp;" "&amp;AL280</f>
+        <v>ADAPAC GEL TOP 0,1% X 30 GR D&amp;M PHARMA ADAPALENO 0,1% gel tópico</v>
+      </c>
+      <c r="BB280">
+        <f t="shared" ref="BB280" si="951">+D280</f>
+        <v>1709585</v>
+      </c>
+      <c r="BC280" t="str">
+        <f t="shared" ref="BC280" si="952">+H280&amp;" "&amp;IF(S280="","x ",S280&amp;" x ")&amp;Y280</f>
+        <v>Adapac 0,1% x 30 g. gel tópico</v>
+      </c>
+      <c r="BD280" s="10">
+        <f t="shared" ref="BD280" si="953">+AE280</f>
         <v>0</v>
+      </c>
+      <c r="BE280" s="3" t="str">
+        <f t="shared" ref="BE280" si="954">+H280</f>
+        <v>Adapac 0,1%</v>
+      </c>
+      <c r="BF280" t="str">
+        <f t="shared" ref="BF280" si="955">+PROPER(M280)</f>
+        <v>Adapaleno</v>
+      </c>
+      <c r="BG280" t="str">
+        <f t="shared" ref="BG280" si="956">+PROPER(N280)</f>
+        <v/>
+      </c>
+      <c r="BH280" t="str">
+        <f t="shared" ref="BH280" si="957">+PROPER(O280)</f>
+        <v/>
+      </c>
+      <c r="BI280" t="str">
+        <f>+IF(AND(X280="ud.",COUNTIF(Hoja2!$I$3:$I$11,Hoja1!Q280)&gt;0),IF(Hoja1!W280=1,VLOOKUP(Hoja1!Q280,Hoja2!$A:$D,3,0),VLOOKUP(Hoja1!Q280,Hoja2!$A:$D,4,0)),IF(AND(X280="ud.",COUNTIF(Hoja2!$I$3:$I$11,Hoja1!Q280)&lt;0),VLOOKUP(Hoja1!Q280,Hoja2!$A:$B,2,0),VLOOKUP(Hoja1!Q280,Hoja2!$A:$B,2,0)))</f>
+        <v>gel tópico</v>
+      </c>
+      <c r="BJ280" t="str">
+        <f t="shared" ref="BJ280" si="958">+G280&amp;" "&amp;S280</f>
+        <v xml:space="preserve">0,1% </v>
+      </c>
+      <c r="BK280">
+        <f t="shared" ref="BK280" si="959">+W280</f>
+        <v>30</v>
+      </c>
+      <c r="BL280" t="str">
+        <f t="shared" ref="BL280" si="960">+X280</f>
+        <v>g.</v>
+      </c>
+      <c r="BO280">
+        <f t="shared" ref="BO280" si="961">+BB280</f>
+        <v>1709585</v>
+      </c>
+      <c r="BP280" t="str">
+        <f t="shared" ref="BP280" si="962">+BC280</f>
+        <v>Adapac 0,1% x 30 g. gel tópico</v>
+      </c>
+      <c r="BQ280" s="10">
+        <f t="shared" ref="BQ280" si="963">+BD280</f>
+        <v>0</v>
+      </c>
+      <c r="BR280" s="3" t="str">
+        <f t="shared" ref="BR280" si="964">+BE280</f>
+        <v>Adapac 0,1%</v>
+      </c>
+      <c r="BS280" t="str">
+        <f t="shared" ref="BS280" si="965">+IF(AND(BG280="",BH280=""),BF280,IF(AND(BG280&lt;&gt;"",BH280=""),BF280&amp;";"&amp;BG280,BF280&amp;";"&amp;BG280&amp;";"&amp;BH280))</f>
+        <v>Adapaleno</v>
+      </c>
+      <c r="BT280" t="str">
+        <f t="shared" ref="BT280" si="966">+BI280</f>
+        <v>gel tópico</v>
+      </c>
+      <c r="BU280" t="str">
+        <f t="shared" ref="BU280" si="967">+BJ280</f>
+        <v xml:space="preserve">0,1% </v>
+      </c>
+      <c r="BV280">
+        <f t="shared" ref="BV280" si="968">+BK280</f>
+        <v>30</v>
+      </c>
+      <c r="BW280" t="str">
+        <f t="shared" ref="BW280" si="969">+BL280</f>
+        <v>g.</v>
+      </c>
+      <c r="BZ280" t="str">
+        <f t="shared" ref="BZ280" si="970">+K280</f>
+        <v>D&amp;M Pharma</v>
+      </c>
+      <c r="CB280">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CC276" xr:uid="{6C510029-7A77-F34A-8A28-8CDA7E85138F}">
+  <autoFilter ref="A1:CC280" xr:uid="{6C510029-7A77-F34A-8A28-8CDA7E85138F}">
     <filterColumn colId="57" showButton="0"/>
     <filterColumn colId="58" showButton="0"/>
   </autoFilter>

</xml_diff>

<commit_message>
actualiza base eliminando item covid
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosyanez/Documents/lista-cb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AA47E1-401C-2147-880B-D042D8DF9A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC16520-C8A5-3C4C-879C-4639C959BDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17620" xr2:uid="{7C1CB140-3D0A-7D4F-AA37-4F2BBC3134C1}"/>
   </bookViews>
@@ -4084,9 +4084,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C510029-7A77-F34A-8A28-8CDA7E85138F}">
   <dimension ref="A1:CC280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CB280" sqref="CB280"/>
+    <sheetView tabSelected="1" topLeftCell="BG1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A246" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BO1" sqref="BO1:CC280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>